<commit_message>
Automate pulling CBO projections
</commit_message>
<xml_diff>
--- a/results/04-2022/comparison-deflators-04-2022.xlsx
+++ b/results/04-2022/comparison-deflators-04-2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">2024 Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 Q2</t>
   </si>
   <si>
     <t xml:space="preserve">Consumption Deflator Growth</t>
@@ -521,16 +518,13 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
       <c r="C2" t="n">
         <v>0.0158</v>
@@ -568,16 +562,13 @@
       <c r="N2" t="n">
         <v>0.0052</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.0052</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="n">
         <v>268.7603</v>
@@ -615,16 +606,13 @@
       <c r="N3" t="n">
         <v>284.262</v>
       </c>
-      <c r="O3" t="n">
-        <v>285.94</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="n">
         <v>0.0427</v>
@@ -662,16 +650,13 @@
       <c r="N4" t="n">
         <v>-0.0068</v>
       </c>
-      <c r="O4" t="n">
-        <v>-0.018</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
         <v>0.0215</v>
@@ -683,42 +668,39 @@
         <v>-0.0285</v>
       </c>
       <c r="F5" t="n">
-        <v>-32.7491</v>
+        <v>-0.0195</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.6459</v>
+        <v>-0.3299</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0175</v>
+        <v>-0.3325</v>
       </c>
       <c r="I5" t="n">
-        <v>3.1367</v>
+        <v>-0.0741</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1041</v>
+        <v>-0.1013</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.3481</v>
+        <v>-0.5253</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1137</v>
+        <v>-0.2696</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0295</v>
+        <v>-0.1041</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.2232</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-0.3641</v>
+        <v>-0.3594</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
         <v>-0.024</v>
@@ -756,16 +738,13 @@
       <c r="N6" t="n">
         <v>-0.0199</v>
       </c>
-      <c r="O6" t="n">
-        <v>-0.0021</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="n">
         <v>-0.2563</v>
@@ -777,42 +756,39 @@
         <v>-0.1454</v>
       </c>
       <c r="F7" t="n">
-        <v>-5.3199</v>
+        <v>0.035</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.1648</v>
+        <v>0.0961</v>
       </c>
       <c r="H7" t="n">
-        <v>-5.1361</v>
+        <v>0.0265</v>
       </c>
       <c r="I7" t="n">
-        <v>-5.1039</v>
+        <v>-0.0182</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0674</v>
+        <v>-0.1833</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.1159</v>
+        <v>-0.1982</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.0642</v>
+        <v>-0.1366</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0538</v>
+        <v>-0.0727</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0026</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.0024</v>
+        <v>0.0373</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="n">
         <v>-0.3402</v>
@@ -824,42 +800,39 @@
         <v>-0.3385</v>
       </c>
       <c r="F8" t="n">
-        <v>7.6763</v>
+        <v>-0.3492</v>
       </c>
       <c r="G8" t="n">
-        <v>7.3901</v>
+        <v>-0.6728</v>
       </c>
       <c r="H8" t="n">
-        <v>3.513</v>
+        <v>-0.6135</v>
       </c>
       <c r="I8" t="n">
-        <v>3.5657</v>
+        <v>-0.3932</v>
       </c>
       <c r="J8" t="n">
-        <v>3.635</v>
+        <v>-0.164</v>
       </c>
       <c r="K8" t="n">
-        <v>3.6718</v>
+        <v>-0.0606</v>
       </c>
       <c r="L8" t="n">
-        <v>3.6962</v>
+        <v>0.0279</v>
       </c>
       <c r="M8" t="n">
-        <v>3.7056</v>
+        <v>0.0134</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="n">
         <v>-0.0224</v>
@@ -871,42 +844,39 @@
         <v>0.1311</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0397</v>
+        <v>0.0908</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0535</v>
+        <v>0.0001</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.2059</v>
+        <v>-0.1887</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0634</v>
+        <v>-0.1233</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0283</v>
+        <v>-0.0615</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0343</v>
+        <v>-0.051</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0217</v>
+        <v>-0.0227</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0319</v>
+        <v>-0.0328</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0647</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-0.0142</v>
+        <v>-0.0657</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="n">
         <v>0.1231</v>
@@ -944,16 +914,13 @@
       <c r="N10" t="n">
         <v>-0.0543</v>
       </c>
-      <c r="O10" t="n">
-        <v>-0.0522</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
         <v>0.0102</v>
@@ -991,16 +958,13 @@
       <c r="N11" t="n">
         <v>0.0055</v>
       </c>
-      <c r="O11" t="n">
-        <v>0.0054</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="n">
         <v>-0.1684</v>
@@ -1012,42 +976,39 @@
         <v>0.3369</v>
       </c>
       <c r="F12" t="n">
-        <v>-7.9542</v>
+        <v>-0.7896</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.2532</v>
+        <v>-0.0738</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.0975</v>
+        <v>-0.9231</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.725</v>
+        <v>-0.5551</v>
       </c>
       <c r="J12" t="n">
-        <v>6.411</v>
+        <v>-0.1269</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.177</v>
+        <v>-0.0269</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0505</v>
+        <v>0.1978</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0744</v>
+        <v>0.07</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0745</v>
-      </c>
-      <c r="O12" t="n">
-        <v>-0.074</v>
+        <v>-0.0117</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="n">
         <v>0.3833</v>
@@ -1059,42 +1020,39 @@
         <v>0.0321</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.2751</v>
+        <v>-0.1262</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.163</v>
+        <v>-0.1489</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1575</v>
+        <v>-0.145</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0453</v>
+        <v>-0.0587</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0367</v>
+        <v>-0.0475</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.6114</v>
+        <v>-0.6157</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.6479</v>
+        <v>-0.6505</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.3129</v>
+        <v>-0.3144</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.1799</v>
-      </c>
-      <c r="O13" t="n">
-        <v>-0.3304</v>
+        <v>-0.1876</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="n">
         <v>0.1724</v>
@@ -1106,42 +1064,39 @@
         <v>-1.074</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.0879</v>
+        <v>-1</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.48</v>
+        <v>-1.494</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.0322</v>
+        <v>-1.0372</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.4232</v>
+        <v>-0.4282</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.3904</v>
+        <v>-0.4163</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.3008</v>
+        <v>-0.3179</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.1495</v>
+        <v>-0.1497</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.0026</v>
+        <v>-0.0069</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0165</v>
-      </c>
-      <c r="O14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="n">
         <v>-2.2613</v>
@@ -1153,42 +1108,39 @@
         <v>-3.2934</v>
       </c>
       <c r="F15" t="n">
-        <v>-73.9633</v>
+        <v>-2.1353</v>
       </c>
       <c r="G15" t="n">
-        <v>1.934</v>
+        <v>-3.4856</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.6928</v>
+        <v>-3.2049</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.4016</v>
+        <v>-2.0618</v>
       </c>
       <c r="J15" t="n">
-        <v>10.7529</v>
+        <v>-2.0979</v>
       </c>
       <c r="K15" t="n">
-        <v>2.911</v>
+        <v>-3.0913</v>
       </c>
       <c r="L15" t="n">
-        <v>4.7215</v>
+        <v>-1.2189</v>
       </c>
       <c r="M15" t="n">
-        <v>5.198</v>
+        <v>-0.6377</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.3809</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-0.4953</v>
+        <v>-0.5157</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="n">
         <v>22741</v>
@@ -1226,16 +1178,13 @@
       <c r="N16" t="n">
         <v>26078.1</v>
       </c>
-      <c r="O16" t="n">
-        <v>26293.7</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="n">
         <v>0.5458</v>
@@ -1247,42 +1196,39 @@
         <v>0.4121</v>
       </c>
       <c r="F17" t="n">
-        <v>-6.3841</v>
+        <v>-0.0125</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.7039</v>
+        <v>-0.1076</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.0169</v>
+        <v>-0.0575</v>
       </c>
       <c r="I17" t="n">
-        <v>3.0568</v>
+        <v>0.1042</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1055</v>
+        <v>0.0911</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.3467</v>
+        <v>-0.3608</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.1123</v>
+        <v>-0.1266</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.0284</v>
+        <v>-0.0416</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.2212</v>
-      </c>
-      <c r="O17" t="n">
-        <v>-0.3622</v>
+        <v>-0.234</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="n">
         <v>0.0048</v>
@@ -1320,16 +1266,13 @@
       <c r="N18" t="n">
         <v>0.0049</v>
       </c>
-      <c r="O18" t="n">
-        <v>0.0048</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" t="n">
         <v>-1.0494</v>
@@ -1367,16 +1310,13 @@
       <c r="N19" t="n">
         <v>-0.0111</v>
       </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" t="n">
         <v>-0.2711</v>
@@ -1414,16 +1354,13 @@
       <c r="N20" t="n">
         <v>0</v>
       </c>
-      <c r="O20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" t="n">
         <v>-0.7397</v>
@@ -1435,42 +1372,39 @@
         <v>-0.8145</v>
       </c>
       <c r="F21" t="n">
-        <v>-36.956</v>
+        <v>0.0734</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7039</v>
+        <v>0.3554</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0169</v>
+        <v>0.2012</v>
       </c>
       <c r="I21" t="n">
-        <v>-3.0568</v>
+        <v>-0.1085</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.1055</v>
+        <v>-0.1431</v>
       </c>
       <c r="K21" t="n">
-        <v>0.3467</v>
+        <v>0.3118</v>
       </c>
       <c r="L21" t="n">
-        <v>0.1123</v>
+        <v>0.0762</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0284</v>
+        <v>0.0023</v>
       </c>
       <c r="N21" t="n">
-        <v>0.2212</v>
-      </c>
-      <c r="O21" t="n">
-        <v>0.3622</v>
+        <v>0.1999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" t="n">
         <v>-0.014</v>
@@ -1508,16 +1442,13 @@
       <c r="N22" t="n">
         <v>-0.0041</v>
       </c>
-      <c r="O22" t="n">
-        <v>-0.0013</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" t="n">
         <v>0.1964</v>
@@ -1529,42 +1460,39 @@
         <v>0.2154</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.7484</v>
+        <v>0.1796</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.8223</v>
+        <v>0.1017</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.9602</v>
+        <v>0.0151</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.9093</v>
+        <v>0.0302</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.0249</v>
+        <v>-0.0065</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.0241</v>
+        <v>-0.0311</v>
       </c>
       <c r="L23" t="n">
-        <v>0.012</v>
+        <v>-0.078</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0017</v>
+        <v>-0.0603</v>
       </c>
       <c r="N23" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0.0003</v>
+        <v>-0.0354</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" t="n">
         <v>-0.0802</v>
@@ -1576,42 +1504,39 @@
         <v>-0.0891</v>
       </c>
       <c r="F24" t="n">
-        <v>4.2624</v>
+        <v>-0.0509</v>
       </c>
       <c r="G24" t="n">
-        <v>4.2267</v>
+        <v>-0.1049</v>
       </c>
       <c r="H24" t="n">
-        <v>2.0944</v>
+        <v>-0.0801</v>
       </c>
       <c r="I24" t="n">
-        <v>2.0469</v>
+        <v>-0.0857</v>
       </c>
       <c r="J24" t="n">
-        <v>2.05</v>
+        <v>-0.0572</v>
       </c>
       <c r="K24" t="n">
-        <v>2.0617</v>
+        <v>-0.0228</v>
       </c>
       <c r="L24" t="n">
-        <v>2.0501</v>
+        <v>-0.0151</v>
       </c>
       <c r="M24" t="n">
-        <v>2.0466</v>
+        <v>0.0017</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0187</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
+        <v>-0.0041</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" t="n">
         <v>0.0178</v>
@@ -1649,16 +1574,13 @@
       <c r="N25" t="n">
         <v>0.0081</v>
       </c>
-      <c r="O25" t="n">
-        <v>0.0081</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" t="n">
         <v>155</v>
@@ -1670,42 +1592,39 @@
         <v>156.3</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>158.1846</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>160.092</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>162.0224</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>163.976</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>165.9532</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>167.9542</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>169.9794</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>172.029</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
+        <v>174.1033</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" t="n">
         <v>0.0069</v>
@@ -1743,16 +1662,13 @@
       <c r="N27" t="n">
         <v>-0.0014</v>
       </c>
-      <c r="O27" t="n">
-        <v>-0.0045</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" t="n">
         <v>-0.2286</v>
@@ -1790,16 +1706,13 @@
       <c r="N28" t="n">
         <v>-0.0011</v>
       </c>
-      <c r="O28" t="n">
-        <v>0.0007</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -1835,18 +1748,15 @@
         <v>0</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -1882,18 +1792,15 @@
         <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -1929,18 +1836,15 @@
         <v>0</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -1952,42 +1856,39 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>-32.7296</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.316</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>0.315</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>3.2108</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0.2054</v>
+        <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>0.1772</v>
+        <v>0</v>
       </c>
       <c r="L32" t="n">
-        <v>0.1559</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
-        <v>0.1336</v>
+        <v>0</v>
       </c>
       <c r="N32" t="n">
-        <v>0.1362</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0.1303</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -2023,18 +1924,15 @@
         <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -2046,42 +1944,39 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>-5.355</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>-5.2609</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>-5.1625</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>-5.0857</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0.1159</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0823</v>
+        <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0724</v>
+        <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0189</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.0347</v>
-      </c>
-      <c r="O34" t="n">
-        <v>-0.0874</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -2093,42 +1988,39 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>8.0255</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>8.0629</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>4.1265</v>
+        <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>3.9589</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>3.799</v>
+        <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>3.7324</v>
+        <v>0</v>
       </c>
       <c r="L35" t="n">
-        <v>3.6683</v>
+        <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>3.6922</v>
+        <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.0054</v>
-      </c>
-      <c r="O35" t="n">
-        <v>-0.0394</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -2140,42 +2032,39 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.1306</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.0536</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.0172</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0599</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0332</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0167</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>0.0009</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0.0009</v>
+        <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0009</v>
-      </c>
-      <c r="O36" t="n">
-        <v>0.0438</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -2211,18 +2100,15 @@
         <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -2258,18 +2144,15 @@
         <v>0</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -2281,42 +2164,39 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>-7.1645</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.1794</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.1744</v>
+        <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.1699</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>6.538</v>
+        <v>0</v>
       </c>
       <c r="K39" t="n">
-        <v>-0.1501</v>
+        <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>-0.1472</v>
+        <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>-0.1444</v>
+        <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>-0.0628</v>
-      </c>
-      <c r="O39" t="n">
-        <v>-0.0616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -2328,42 +2208,39 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>-0.1489</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.014</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>-0.0124</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0134</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0109</v>
+        <v>0</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0042</v>
+        <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>0.0026</v>
+        <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0015</v>
+        <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0078</v>
-      </c>
-      <c r="O40" t="n">
-        <v>0.0029</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -2375,42 +2252,39 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.0879</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.014</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0051</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0.0259</v>
+        <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>0.0171</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="M41" t="n">
-        <v>0.0043</v>
+        <v>0</v>
       </c>
       <c r="N41" t="n">
-        <v>0.0165</v>
-      </c>
-      <c r="O41" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -2422,42 +2296,39 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>-71.828</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>5.4196</v>
+        <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.4878</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>-0.3398</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>12.8508</v>
+        <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>6.0023</v>
+        <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>5.9404</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
-        <v>5.8358</v>
+        <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>0.1348</v>
-      </c>
-      <c r="O42" t="n">
-        <v>0.5537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -2493,18 +2364,15 @@
         <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -2516,42 +2384,39 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>-6.3716</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.5963</v>
+        <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0406</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>2.9525</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0144</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0141</v>
+        <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0143</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0133</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0128</v>
-      </c>
-      <c r="O44" t="n">
-        <v>0.0122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -2587,18 +2452,15 @@
         <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>0</v>
-      </c>
-      <c r="O45" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -2634,18 +2496,15 @@
         <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
-      </c>
-      <c r="O46" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -2681,18 +2540,15 @@
         <v>0</v>
       </c>
       <c r="N47" t="n">
-        <v>0</v>
-      </c>
-      <c r="O47" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -2704,42 +2560,39 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>-37.0294</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0.3486</v>
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.1843</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>-2.9482</v>
+        <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>0.0376</v>
+        <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>0.0349</v>
+        <v>0</v>
       </c>
       <c r="L48" t="n">
-        <v>0.0362</v>
+        <v>0</v>
       </c>
       <c r="M48" t="n">
-        <v>0.0261</v>
+        <v>0</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0214</v>
-      </c>
-      <c r="O48" t="n">
-        <v>0.5632</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -2775,18 +2628,15 @@
         <v>0</v>
       </c>
       <c r="N49" t="n">
-        <v>0</v>
-      </c>
-      <c r="O49" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -2798,42 +2648,39 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.928</v>
+        <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.9241</v>
+        <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.9754</v>
+        <v>0</v>
       </c>
       <c r="I50" t="n">
-        <v>-0.9395</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>-0.0183</v>
+        <v>0</v>
       </c>
       <c r="K50" t="n">
-        <v>0.007</v>
+        <v>0</v>
       </c>
       <c r="L50" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="M50" t="n">
-        <v>0.062</v>
+        <v>0</v>
       </c>
       <c r="N50" t="n">
-        <v>0.0364</v>
-      </c>
-      <c r="O50" t="n">
-        <v>0.0113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -2845,42 +2692,39 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>4.3134</v>
+        <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>4.3316</v>
+        <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>2.1745</v>
+        <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>2.1326</v>
+        <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>2.1072</v>
+        <v>0</v>
       </c>
       <c r="K51" t="n">
-        <v>2.0846</v>
+        <v>0</v>
       </c>
       <c r="L51" t="n">
-        <v>2.0652</v>
+        <v>0</v>
       </c>
       <c r="M51" t="n">
-        <v>2.0448</v>
+        <v>0</v>
       </c>
       <c r="N51" t="n">
-        <v>0.0228</v>
-      </c>
-      <c r="O51" t="n">
-        <v>-0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -2916,18 +2760,15 @@
         <v>0</v>
       </c>
       <c r="N52" t="n">
-        <v>0</v>
-      </c>
-      <c r="O52" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -2939,42 +2780,39 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>-158.1846</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>-160.092</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>-162.0224</v>
+        <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>-163.976</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>-165.9532</v>
+        <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>-167.9542</v>
+        <v>0</v>
       </c>
       <c r="L53" t="n">
-        <v>-169.9794</v>
+        <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>-172.029</v>
+        <v>0</v>
       </c>
       <c r="N53" t="n">
-        <v>-174.1033</v>
-      </c>
-      <c r="O53" t="n">
-        <v>-176.2026</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -3010,19 +2848,16 @@
         <v>0</v>
       </c>
       <c r="N54" t="n">
-        <v>0</v>
-      </c>
-      <c r="O54" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
         <v>42</v>
       </c>
-      <c r="B55" t="s">
-        <v>43</v>
-      </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
@@ -3057,18 +2892,15 @@
         <v>0</v>
       </c>
       <c r="N55" t="n">
-        <v>0</v>
-      </c>
-      <c r="O55" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" t="n">
         <v>0.0158</v>
@@ -3106,16 +2938,13 @@
       <c r="N56" t="n">
         <v>0.0052</v>
       </c>
-      <c r="O56" t="n">
-        <v>0.0052</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C57" t="n">
         <v>268.7603</v>
@@ -3153,16 +2982,13 @@
       <c r="N57" t="n">
         <v>284.262</v>
       </c>
-      <c r="O57" t="n">
-        <v>285.94</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C58" t="n">
         <v>0.0427</v>
@@ -3200,16 +3026,13 @@
       <c r="N58" t="n">
         <v>-0.0068</v>
       </c>
-      <c r="O58" t="n">
-        <v>-0.018</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C59" t="n">
         <v>0.0215</v>
@@ -3247,16 +3070,13 @@
       <c r="N59" t="n">
         <v>-0.3594</v>
       </c>
-      <c r="O59" t="n">
-        <v>-0.4944</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C60" t="n">
         <v>-0.024</v>
@@ -3294,16 +3114,13 @@
       <c r="N60" t="n">
         <v>-0.0199</v>
       </c>
-      <c r="O60" t="n">
-        <v>-0.0021</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61" t="n">
         <v>-0.2563</v>
@@ -3341,16 +3158,13 @@
       <c r="N61" t="n">
         <v>0.0373</v>
       </c>
-      <c r="O61" t="n">
-        <v>0.0898</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C62" t="n">
         <v>-0.3402</v>
@@ -3388,16 +3202,13 @@
       <c r="N62" t="n">
         <v>0.0054</v>
       </c>
-      <c r="O62" t="n">
-        <v>0.0394</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C63" t="n">
         <v>-0.0224</v>
@@ -3435,16 +3246,13 @@
       <c r="N63" t="n">
         <v>-0.0657</v>
       </c>
-      <c r="O63" t="n">
-        <v>-0.058</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B64" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C64" t="n">
         <v>0.1231</v>
@@ -3482,16 +3290,13 @@
       <c r="N64" t="n">
         <v>-0.0543</v>
       </c>
-      <c r="O64" t="n">
-        <v>-0.0522</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C65" t="n">
         <v>0.0102</v>
@@ -3529,16 +3334,13 @@
       <c r="N65" t="n">
         <v>0.0055</v>
       </c>
-      <c r="O65" t="n">
-        <v>0.0054</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C66" t="n">
         <v>-0.1684</v>
@@ -3576,16 +3378,13 @@
       <c r="N66" t="n">
         <v>-0.0117</v>
       </c>
-      <c r="O66" t="n">
-        <v>-0.0124</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C67" t="n">
         <v>0.3833</v>
@@ -3623,16 +3422,13 @@
       <c r="N67" t="n">
         <v>-0.1876</v>
       </c>
-      <c r="O67" t="n">
-        <v>-0.3333</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C68" t="n">
         <v>0.1724</v>
@@ -3670,16 +3466,13 @@
       <c r="N68" t="n">
         <v>0</v>
       </c>
-      <c r="O68" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C69" t="n">
         <v>-2.2613</v>
@@ -3717,16 +3510,13 @@
       <c r="N69" t="n">
         <v>-0.5157</v>
       </c>
-      <c r="O69" t="n">
-        <v>-1.0491</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C70" t="n">
         <v>22741</v>
@@ -3764,16 +3554,13 @@
       <c r="N70" t="n">
         <v>26078.1</v>
       </c>
-      <c r="O70" t="n">
-        <v>26293.7</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C71" t="n">
         <v>0.5458</v>
@@ -3811,16 +3598,13 @@
       <c r="N71" t="n">
         <v>-0.234</v>
       </c>
-      <c r="O71" t="n">
-        <v>-0.3744</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C72" t="n">
         <v>0.0048</v>
@@ -3858,16 +3642,13 @@
       <c r="N72" t="n">
         <v>0.0049</v>
       </c>
-      <c r="O72" t="n">
-        <v>0.0048</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C73" t="n">
         <v>-1.0494</v>
@@ -3905,16 +3686,13 @@
       <c r="N73" t="n">
         <v>-0.0111</v>
       </c>
-      <c r="O73" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C74" t="n">
         <v>-0.2711</v>
@@ -3952,16 +3730,13 @@
       <c r="N74" t="n">
         <v>0</v>
       </c>
-      <c r="O74" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C75" t="n">
         <v>-0.7397</v>
@@ -3999,16 +3774,13 @@
       <c r="N75" t="n">
         <v>0.1999</v>
       </c>
-      <c r="O75" t="n">
-        <v>-0.2011</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C76" t="n">
         <v>-0.014</v>
@@ -4046,16 +3818,13 @@
       <c r="N76" t="n">
         <v>-0.0041</v>
       </c>
-      <c r="O76" t="n">
-        <v>-0.0013</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C77" t="n">
         <v>0.1964</v>
@@ -4093,16 +3862,13 @@
       <c r="N77" t="n">
         <v>-0.0354</v>
       </c>
-      <c r="O77" t="n">
-        <v>-0.011</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C78" t="n">
         <v>-0.0802</v>
@@ -4140,16 +3906,13 @@
       <c r="N78" t="n">
         <v>-0.0041</v>
       </c>
-      <c r="O78" t="n">
-        <v>0.005</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C79" t="n">
         <v>0.0178</v>
@@ -4187,16 +3950,13 @@
       <c r="N79" t="n">
         <v>0.0081</v>
       </c>
-      <c r="O79" t="n">
-        <v>0.0081</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C80" t="n">
         <v>155</v>
@@ -4234,16 +3994,13 @@
       <c r="N80" t="n">
         <v>174.1033</v>
       </c>
-      <c r="O80" t="n">
-        <v>176.2026</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B81" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C81" t="n">
         <v>0.0069</v>
@@ -4281,16 +4038,13 @@
       <c r="N81" t="n">
         <v>-0.0014</v>
       </c>
-      <c r="O81" t="n">
-        <v>-0.0045</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C82" t="n">
         <v>-0.2286</v>
@@ -4327,9 +4081,6 @@
       </c>
       <c r="N82" t="n">
         <v>-0.0011</v>
-      </c>
-      <c r="O82" t="n">
-        <v>0.0007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing rendring index on a branch
</commit_message>
<xml_diff>
--- a/results/04-2022/comparison-deflators-04-2022.xlsx
+++ b/results/04-2022/comparison-deflators-04-2022.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t xml:space="preserve">2024 Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 Q2</t>
   </si>
   <si>
     <t xml:space="preserve">Consumption Deflator Growth</t>
@@ -518,13 +521,16 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
         <v>0.0158</v>
@@ -562,13 +568,16 @@
       <c r="N2" t="n">
         <v>0.0052</v>
       </c>
+      <c r="O2" t="n">
+        <v>0.0052</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3" t="n">
         <v>268.7603</v>
@@ -606,13 +615,16 @@
       <c r="N3" t="n">
         <v>284.262</v>
       </c>
+      <c r="O3" t="n">
+        <v>285.94</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
         <v>0.0427</v>
@@ -650,13 +662,16 @@
       <c r="N4" t="n">
         <v>-0.0068</v>
       </c>
+      <c r="O4" t="n">
+        <v>-0.018</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="n">
         <v>0.0215</v>
@@ -668,39 +683,42 @@
         <v>-0.0285</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.0195</v>
+        <v>-32.7491</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.3299</v>
+        <v>-0.6459</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.3325</v>
+        <v>-0.0175</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0741</v>
+        <v>3.1367</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.1013</v>
+        <v>0.1041</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.5253</v>
+        <v>-0.3481</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.2696</v>
+        <v>-0.1137</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.1041</v>
+        <v>0.0295</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.3594</v>
+        <v>-0.2232</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-0.3641</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
         <v>-0.024</v>
@@ -738,13 +756,16 @@
       <c r="N6" t="n">
         <v>-0.0199</v>
       </c>
+      <c r="O6" t="n">
+        <v>-0.0021</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
         <v>-0.2563</v>
@@ -756,39 +777,42 @@
         <v>-0.1454</v>
       </c>
       <c r="F7" t="n">
-        <v>0.035</v>
+        <v>-5.3199</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0961</v>
+        <v>-5.1648</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0265</v>
+        <v>-5.1361</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.0182</v>
+        <v>-5.1039</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1833</v>
+        <v>-0.0674</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.1982</v>
+        <v>-0.1159</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.1366</v>
+        <v>-0.0642</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0727</v>
+        <v>-0.0538</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0373</v>
+        <v>0.0026</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.0024</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
         <v>-0.3402</v>
@@ -800,39 +824,42 @@
         <v>-0.3385</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.3492</v>
+        <v>7.6763</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.6728</v>
+        <v>7.3901</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.6135</v>
+        <v>3.513</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.3932</v>
+        <v>3.5657</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.164</v>
+        <v>3.635</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0606</v>
+        <v>3.6718</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0279</v>
+        <v>3.6962</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0134</v>
+        <v>3.7056</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0054</v>
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="n">
         <v>-0.0224</v>
@@ -844,39 +871,42 @@
         <v>0.1311</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0908</v>
+        <v>-0.0397</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0001</v>
+        <v>-0.0535</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1887</v>
+        <v>-0.2059</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.1233</v>
+        <v>-0.0634</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0615</v>
+        <v>-0.0283</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.051</v>
+        <v>-0.0343</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0227</v>
+        <v>-0.0217</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0328</v>
+        <v>-0.0319</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0657</v>
+        <v>-0.0647</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-0.0142</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="n">
         <v>0.1231</v>
@@ -914,13 +944,16 @@
       <c r="N10" t="n">
         <v>-0.0543</v>
       </c>
+      <c r="O10" t="n">
+        <v>-0.0522</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" t="n">
         <v>0.0102</v>
@@ -958,13 +991,16 @@
       <c r="N11" t="n">
         <v>0.0055</v>
       </c>
+      <c r="O11" t="n">
+        <v>0.0054</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" t="n">
         <v>-0.1684</v>
@@ -976,39 +1012,42 @@
         <v>0.3369</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.7896</v>
+        <v>-7.9542</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.0738</v>
+        <v>-0.2532</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.9231</v>
+        <v>-1.0975</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.5551</v>
+        <v>-0.725</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.1269</v>
+        <v>6.411</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0269</v>
+        <v>-0.177</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1978</v>
+        <v>0.0505</v>
       </c>
       <c r="M12" t="n">
-        <v>0.07</v>
+        <v>-0.0744</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0117</v>
+        <v>-0.0745</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-0.074</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="n">
         <v>0.3833</v>
@@ -1020,39 +1059,42 @@
         <v>0.0321</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1262</v>
+        <v>-0.2751</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1489</v>
+        <v>-0.163</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.145</v>
+        <v>-0.1575</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0587</v>
+        <v>-0.0453</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0475</v>
+        <v>-0.0367</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.6157</v>
+        <v>-0.6114</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.6505</v>
+        <v>-0.6479</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.3144</v>
+        <v>-0.3129</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.1876</v>
+        <v>-0.1799</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-0.3304</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="n">
         <v>0.1724</v>
@@ -1064,39 +1106,42 @@
         <v>-1.074</v>
       </c>
       <c r="F14" t="n">
-        <v>-1</v>
+        <v>-1.0879</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.494</v>
+        <v>-1.48</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.0372</v>
+        <v>-1.0322</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.4282</v>
+        <v>-0.4232</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.4163</v>
+        <v>-0.3904</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.3179</v>
+        <v>-0.3008</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.1497</v>
+        <v>-0.1495</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.0069</v>
+        <v>-0.0026</v>
       </c>
       <c r="N14" t="n">
+        <v>0.0165</v>
+      </c>
+      <c r="O14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="n">
         <v>-2.2613</v>
@@ -1108,39 +1153,42 @@
         <v>-3.2934</v>
       </c>
       <c r="F15" t="n">
-        <v>-2.1353</v>
+        <v>-73.9633</v>
       </c>
       <c r="G15" t="n">
-        <v>-3.4856</v>
+        <v>1.934</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.2049</v>
+        <v>-3.6928</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.0618</v>
+        <v>-2.4016</v>
       </c>
       <c r="J15" t="n">
-        <v>-2.0979</v>
+        <v>10.7529</v>
       </c>
       <c r="K15" t="n">
-        <v>-3.0913</v>
+        <v>2.911</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.2189</v>
+        <v>4.7215</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.6377</v>
+        <v>5.198</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.5157</v>
+        <v>-0.3809</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-0.4953</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" t="n">
         <v>22741</v>
@@ -1178,13 +1226,16 @@
       <c r="N16" t="n">
         <v>26078.1</v>
       </c>
+      <c r="O16" t="n">
+        <v>26293.7</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" t="n">
         <v>0.5458</v>
@@ -1196,39 +1247,42 @@
         <v>0.4121</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.0125</v>
+        <v>-6.3841</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.1076</v>
+        <v>-0.7039</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.0575</v>
+        <v>-0.0169</v>
       </c>
       <c r="I17" t="n">
-        <v>0.1042</v>
+        <v>3.0568</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0911</v>
+        <v>0.1055</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.3608</v>
+        <v>-0.3467</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.1266</v>
+        <v>-0.1123</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.0416</v>
+        <v>-0.0284</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.234</v>
+        <v>-0.2212</v>
+      </c>
+      <c r="O17" t="n">
+        <v>-0.3622</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" t="n">
         <v>0.0048</v>
@@ -1266,13 +1320,16 @@
       <c r="N18" t="n">
         <v>0.0049</v>
       </c>
+      <c r="O18" t="n">
+        <v>0.0048</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" t="n">
         <v>-1.0494</v>
@@ -1310,13 +1367,16 @@
       <c r="N19" t="n">
         <v>-0.0111</v>
       </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" t="n">
         <v>-0.2711</v>
@@ -1354,13 +1414,16 @@
       <c r="N20" t="n">
         <v>0</v>
       </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" t="n">
         <v>-0.7397</v>
@@ -1372,39 +1435,42 @@
         <v>-0.8145</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0734</v>
+        <v>-36.956</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3554</v>
+        <v>0.7039</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2012</v>
+        <v>0.0169</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.1085</v>
+        <v>-3.0568</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.1431</v>
+        <v>-0.1055</v>
       </c>
       <c r="K21" t="n">
-        <v>0.3118</v>
+        <v>0.3467</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0762</v>
+        <v>0.1123</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0023</v>
+        <v>0.0284</v>
       </c>
       <c r="N21" t="n">
-        <v>0.1999</v>
+        <v>0.2212</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.3622</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" t="n">
         <v>-0.014</v>
@@ -1442,13 +1508,16 @@
       <c r="N22" t="n">
         <v>-0.0041</v>
       </c>
+      <c r="O22" t="n">
+        <v>-0.0013</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" t="n">
         <v>0.1964</v>
@@ -1460,39 +1529,42 @@
         <v>0.2154</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1796</v>
+        <v>-0.7484</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1017</v>
+        <v>-0.8223</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0151</v>
+        <v>-0.9602</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0302</v>
+        <v>-0.9093</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.0065</v>
+        <v>-0.0249</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.0311</v>
+        <v>-0.0241</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.078</v>
+        <v>0.012</v>
       </c>
       <c r="M23" t="n">
-        <v>-0.0603</v>
+        <v>0.0017</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.0354</v>
+        <v>0.001</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.0003</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" t="n">
         <v>-0.0802</v>
@@ -1504,39 +1576,42 @@
         <v>-0.0891</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.0509</v>
+        <v>4.2624</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.1049</v>
+        <v>4.2267</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.0801</v>
+        <v>2.0944</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.0857</v>
+        <v>2.0469</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.0572</v>
+        <v>2.05</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0228</v>
+        <v>2.0617</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.0151</v>
+        <v>2.0501</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0017</v>
+        <v>2.0466</v>
       </c>
       <c r="N24" t="n">
-        <v>-0.0041</v>
+        <v>0.0187</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" t="n">
         <v>0.0178</v>
@@ -1574,13 +1649,16 @@
       <c r="N25" t="n">
         <v>0.0081</v>
       </c>
+      <c r="O25" t="n">
+        <v>0.0081</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" t="n">
         <v>155</v>
@@ -1592,39 +1670,42 @@
         <v>156.3</v>
       </c>
       <c r="F26" t="n">
-        <v>158.1846</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>160.092</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>162.0224</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>163.976</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>165.9532</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>167.9542</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>169.9794</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>172.029</v>
+        <v>0</v>
       </c>
       <c r="N26" t="n">
-        <v>174.1033</v>
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" t="n">
         <v>0.0069</v>
@@ -1662,13 +1743,16 @@
       <c r="N27" t="n">
         <v>-0.0014</v>
       </c>
+      <c r="O27" t="n">
+        <v>-0.0045</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28" t="n">
         <v>-0.2286</v>
@@ -1706,13 +1790,16 @@
       <c r="N28" t="n">
         <v>-0.0011</v>
       </c>
+      <c r="O28" t="n">
+        <v>0.0007</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -1748,15 +1835,18 @@
         <v>0</v>
       </c>
       <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -1792,15 +1882,18 @@
         <v>0</v>
       </c>
       <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -1836,15 +1929,18 @@
         <v>0</v>
       </c>
       <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -1856,39 +1952,42 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>-32.7296</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>-0.316</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>0.315</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>3.2108</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>0.2054</v>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>0.1772</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>0.1559</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>0.1336</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>0.1362</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.1303</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -1924,15 +2023,18 @@
         <v>0</v>
       </c>
       <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -1944,39 +2046,42 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>-5.355</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>-5.2609</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>-5.1625</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>-5.0857</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>0.1159</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>0.0823</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>0.0724</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>0.0189</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>-0.0347</v>
+      </c>
+      <c r="O34" t="n">
+        <v>-0.0874</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1988,39 +2093,42 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>8.0255</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>8.0629</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>4.1265</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>3.9589</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>3.799</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>3.7324</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>3.6683</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>3.6922</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>-0.0054</v>
+      </c>
+      <c r="O35" t="n">
+        <v>-0.0394</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -2032,39 +2140,42 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>-0.1306</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>-0.0536</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>-0.0172</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>0.0599</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>0.0332</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>0.0167</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>0.0009</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>0.0009</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>0.0009</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.0438</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -2100,15 +2211,18 @@
         <v>0</v>
       </c>
       <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -2144,15 +2258,18 @@
         <v>0</v>
       </c>
       <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -2164,39 +2281,42 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>-7.1645</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>-0.1794</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>-0.1744</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>-0.1699</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>6.538</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>-0.1501</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>-0.1472</v>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>-0.1444</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>-0.0628</v>
+      </c>
+      <c r="O39" t="n">
+        <v>-0.0616</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -2208,39 +2328,42 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>-0.1489</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>-0.014</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>-0.0124</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.0134</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>0.0109</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>0.0042</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>0.0026</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>0.0078</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.0029</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -2252,39 +2375,42 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>-0.0879</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>0.014</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>0.0051</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>0.0259</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>0.0171</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>0.0043</v>
       </c>
       <c r="N41" t="n">
+        <v>0.0165</v>
+      </c>
+      <c r="O41" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -2296,39 +2422,42 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>-71.828</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>5.4196</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>-0.4878</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>-0.3398</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>12.8508</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>6.0023</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>5.9404</v>
       </c>
       <c r="M42" t="n">
-        <v>0</v>
+        <v>5.8358</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>0.1348</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.5537</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -2364,15 +2493,18 @@
         <v>0</v>
       </c>
       <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -2384,39 +2516,42 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>-6.3716</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>-0.5963</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>0.0406</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>2.9525</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>0.0144</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>0.0141</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>0.0143</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>0.0133</v>
       </c>
       <c r="N44" t="n">
-        <v>0</v>
+        <v>0.0128</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.0122</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -2452,15 +2587,18 @@
         <v>0</v>
       </c>
       <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -2496,15 +2634,18 @@
         <v>0</v>
       </c>
       <c r="N46" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -2540,15 +2681,18 @@
         <v>0</v>
       </c>
       <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -2560,39 +2704,42 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>-37.0294</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>0.3486</v>
       </c>
       <c r="H48" t="n">
-        <v>0</v>
+        <v>-0.1843</v>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>-2.9482</v>
       </c>
       <c r="J48" t="n">
-        <v>0</v>
+        <v>0.0376</v>
       </c>
       <c r="K48" t="n">
-        <v>0</v>
+        <v>0.0349</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>0.0362</v>
       </c>
       <c r="M48" t="n">
-        <v>0</v>
+        <v>0.0261</v>
       </c>
       <c r="N48" t="n">
-        <v>0</v>
+        <v>0.0214</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.5632</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -2628,15 +2775,18 @@
         <v>0</v>
       </c>
       <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -2648,39 +2798,42 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>-0.928</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>-0.9241</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>-0.9754</v>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>-0.9395</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>-0.0183</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
       <c r="L50" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="M50" t="n">
-        <v>0</v>
+        <v>0.062</v>
       </c>
       <c r="N50" t="n">
-        <v>0</v>
+        <v>0.0364</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.0113</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -2692,39 +2845,42 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
+        <v>4.3134</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>4.3316</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>2.1745</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>2.1326</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>2.1072</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>2.0846</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>2.0652</v>
       </c>
       <c r="M51" t="n">
-        <v>0</v>
+        <v>2.0448</v>
       </c>
       <c r="N51" t="n">
-        <v>0</v>
+        <v>0.0228</v>
+      </c>
+      <c r="O51" t="n">
+        <v>-0.005</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -2760,15 +2916,18 @@
         <v>0</v>
       </c>
       <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -2780,39 +2939,42 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>-158.1846</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>-160.092</v>
       </c>
       <c r="H53" t="n">
-        <v>0</v>
+        <v>-162.0224</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>-163.976</v>
       </c>
       <c r="J53" t="n">
-        <v>0</v>
+        <v>-165.9532</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>-167.9542</v>
       </c>
       <c r="L53" t="n">
-        <v>0</v>
+        <v>-169.9794</v>
       </c>
       <c r="M53" t="n">
-        <v>0</v>
+        <v>-172.029</v>
       </c>
       <c r="N53" t="n">
-        <v>0</v>
+        <v>-174.1033</v>
+      </c>
+      <c r="O53" t="n">
+        <v>-176.2026</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B54" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -2848,15 +3010,18 @@
         <v>0</v>
       </c>
       <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
@@ -2892,15 +3057,18 @@
         <v>0</v>
       </c>
       <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C56" t="n">
         <v>0.0158</v>
@@ -2938,13 +3106,16 @@
       <c r="N56" t="n">
         <v>0.0052</v>
       </c>
+      <c r="O56" t="n">
+        <v>0.0052</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C57" t="n">
         <v>268.7603</v>
@@ -2982,13 +3153,16 @@
       <c r="N57" t="n">
         <v>284.262</v>
       </c>
+      <c r="O57" t="n">
+        <v>285.94</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C58" t="n">
         <v>0.0427</v>
@@ -3026,13 +3200,16 @@
       <c r="N58" t="n">
         <v>-0.0068</v>
       </c>
+      <c r="O58" t="n">
+        <v>-0.018</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C59" t="n">
         <v>0.0215</v>
@@ -3070,13 +3247,16 @@
       <c r="N59" t="n">
         <v>-0.3594</v>
       </c>
+      <c r="O59" t="n">
+        <v>-0.4944</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C60" t="n">
         <v>-0.024</v>
@@ -3114,13 +3294,16 @@
       <c r="N60" t="n">
         <v>-0.0199</v>
       </c>
+      <c r="O60" t="n">
+        <v>-0.0021</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C61" t="n">
         <v>-0.2563</v>
@@ -3158,13 +3341,16 @@
       <c r="N61" t="n">
         <v>0.0373</v>
       </c>
+      <c r="O61" t="n">
+        <v>0.0898</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C62" t="n">
         <v>-0.3402</v>
@@ -3202,13 +3388,16 @@
       <c r="N62" t="n">
         <v>0.0054</v>
       </c>
+      <c r="O62" t="n">
+        <v>0.0394</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C63" t="n">
         <v>-0.0224</v>
@@ -3246,13 +3435,16 @@
       <c r="N63" t="n">
         <v>-0.0657</v>
       </c>
+      <c r="O63" t="n">
+        <v>-0.058</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C64" t="n">
         <v>0.1231</v>
@@ -3290,13 +3482,16 @@
       <c r="N64" t="n">
         <v>-0.0543</v>
       </c>
+      <c r="O64" t="n">
+        <v>-0.0522</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C65" t="n">
         <v>0.0102</v>
@@ -3334,13 +3529,16 @@
       <c r="N65" t="n">
         <v>0.0055</v>
       </c>
+      <c r="O65" t="n">
+        <v>0.0054</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C66" t="n">
         <v>-0.1684</v>
@@ -3378,13 +3576,16 @@
       <c r="N66" t="n">
         <v>-0.0117</v>
       </c>
+      <c r="O66" t="n">
+        <v>-0.0124</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C67" t="n">
         <v>0.3833</v>
@@ -3422,13 +3623,16 @@
       <c r="N67" t="n">
         <v>-0.1876</v>
       </c>
+      <c r="O67" t="n">
+        <v>-0.3333</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C68" t="n">
         <v>0.1724</v>
@@ -3466,13 +3670,16 @@
       <c r="N68" t="n">
         <v>0</v>
       </c>
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C69" t="n">
         <v>-2.2613</v>
@@ -3510,13 +3717,16 @@
       <c r="N69" t="n">
         <v>-0.5157</v>
       </c>
+      <c r="O69" t="n">
+        <v>-1.0491</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C70" t="n">
         <v>22741</v>
@@ -3554,13 +3764,16 @@
       <c r="N70" t="n">
         <v>26078.1</v>
       </c>
+      <c r="O70" t="n">
+        <v>26293.7</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C71" t="n">
         <v>0.5458</v>
@@ -3598,13 +3811,16 @@
       <c r="N71" t="n">
         <v>-0.234</v>
       </c>
+      <c r="O71" t="n">
+        <v>-0.3744</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C72" t="n">
         <v>0.0048</v>
@@ -3642,13 +3858,16 @@
       <c r="N72" t="n">
         <v>0.0049</v>
       </c>
+      <c r="O72" t="n">
+        <v>0.0048</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C73" t="n">
         <v>-1.0494</v>
@@ -3686,13 +3905,16 @@
       <c r="N73" t="n">
         <v>-0.0111</v>
       </c>
+      <c r="O73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C74" t="n">
         <v>-0.2711</v>
@@ -3730,13 +3952,16 @@
       <c r="N74" t="n">
         <v>0</v>
       </c>
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C75" t="n">
         <v>-0.7397</v>
@@ -3774,13 +3999,16 @@
       <c r="N75" t="n">
         <v>0.1999</v>
       </c>
+      <c r="O75" t="n">
+        <v>-0.2011</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C76" t="n">
         <v>-0.014</v>
@@ -3818,13 +4046,16 @@
       <c r="N76" t="n">
         <v>-0.0041</v>
       </c>
+      <c r="O76" t="n">
+        <v>-0.0013</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C77" t="n">
         <v>0.1964</v>
@@ -3862,13 +4093,16 @@
       <c r="N77" t="n">
         <v>-0.0354</v>
       </c>
+      <c r="O77" t="n">
+        <v>-0.011</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C78" t="n">
         <v>-0.0802</v>
@@ -3906,13 +4140,16 @@
       <c r="N78" t="n">
         <v>-0.0041</v>
       </c>
+      <c r="O78" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C79" t="n">
         <v>0.0178</v>
@@ -3950,13 +4187,16 @@
       <c r="N79" t="n">
         <v>0.0081</v>
       </c>
+      <c r="O79" t="n">
+        <v>0.0081</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B80" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C80" t="n">
         <v>155</v>
@@ -3994,13 +4234,16 @@
       <c r="N80" t="n">
         <v>174.1033</v>
       </c>
+      <c r="O80" t="n">
+        <v>176.2026</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C81" t="n">
         <v>0.0069</v>
@@ -4038,13 +4281,16 @@
       <c r="N81" t="n">
         <v>-0.0014</v>
       </c>
+      <c r="O81" t="n">
+        <v>-0.0045</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C82" t="n">
         <v>-0.2286</v>
@@ -4081,6 +4327,9 @@
       </c>
       <c r="N82" t="n">
         <v>-0.0011</v>
+      </c>
+      <c r="O82" t="n">
+        <v>0.0007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
April update with Omnibus
</commit_message>
<xml_diff>
--- a/results/04-2022/comparison-deflators-04-2022.xlsx
+++ b/results/04-2022/comparison-deflators-04-2022.xlsx
@@ -542,34 +542,34 @@
         <v>0.0155</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0046</v>
+        <v>0.0171</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0051</v>
+        <v>0.0147</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0051</v>
+        <v>0.0123</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0051</v>
+        <v>0.0099</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0052</v>
+        <v>0.0099</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0052</v>
+        <v>0.0086</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0052</v>
+        <v>0.0074</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0052</v>
+        <v>0.0074</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0052</v>
+        <v>0.0074</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0052</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="3">
@@ -589,7 +589,7 @@
         <v>278.4133</v>
       </c>
       <c r="F3" t="n">
-        <v>271.441</v>
+        <v>284.6077</v>
       </c>
       <c r="G3" t="n">
         <v>273.2</v>
@@ -636,34 +636,34 @@
         <v>0.0482</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.0339</v>
+        <v>-0.0348</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0277</v>
+        <v>0.0258</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0269</v>
+        <v>0.0254</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.0366</v>
+        <v>-0.0381</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.0359</v>
+        <v>-0.0371</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0003</v>
+        <v>-0.0008</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0002</v>
+        <v>-0.0008</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.0069</v>
+        <v>-0.0079</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0068</v>
+        <v>-0.0078</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.018</v>
+        <v>-0.019</v>
       </c>
     </row>
     <row r="5">
@@ -677,40 +677,40 @@
         <v>0.0215</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0798</v>
+        <v>-0.5195</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.0285</v>
+        <v>-0.0178</v>
       </c>
       <c r="F5" t="n">
-        <v>-32.7491</v>
+        <v>-0.1503</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.6459</v>
+        <v>-0.2238</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.0175</v>
+        <v>-0.1907</v>
       </c>
       <c r="I5" t="n">
-        <v>3.1367</v>
+        <v>-0.2226</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1041</v>
+        <v>-0.2546</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.3481</v>
+        <v>-0.2876</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.1137</v>
+        <v>-0.3058</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0295</v>
+        <v>-0.2194</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.2232</v>
+        <v>-1.7597</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.3641</v>
+        <v>-0.558</v>
       </c>
     </row>
     <row r="6">
@@ -730,34 +730,34 @@
         <v>-0.0151</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0221</v>
+        <v>-0.0201</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0195</v>
+        <v>-0.0159</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.0274</v>
+        <v>-0.0228</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0197</v>
+        <v>-0.0145</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0601</v>
+        <v>-0.0541</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0646</v>
+        <v>-0.0581</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0475</v>
+        <v>-0.0408</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0352</v>
+        <v>-0.0281</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0199</v>
+        <v>-0.0124</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.0021</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="7">
@@ -777,34 +777,34 @@
         <v>-0.1454</v>
       </c>
       <c r="F7" t="n">
-        <v>-5.3199</v>
+        <v>0.0636</v>
       </c>
       <c r="G7" t="n">
-        <v>-5.1648</v>
+        <v>0.0415</v>
       </c>
       <c r="H7" t="n">
-        <v>-5.1361</v>
+        <v>-0.0141</v>
       </c>
       <c r="I7" t="n">
-        <v>-5.1039</v>
+        <v>-0.0841</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0674</v>
+        <v>-0.3014</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.1159</v>
+        <v>-0.2546</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.0642</v>
+        <v>-0.2169</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0538</v>
+        <v>-0.1914</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0026</v>
+        <v>-0.067</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0024</v>
+        <v>-0.0005</v>
       </c>
     </row>
     <row r="8">
@@ -824,34 +824,34 @@
         <v>-0.3385</v>
       </c>
       <c r="F8" t="n">
-        <v>7.6763</v>
+        <v>-0.2122</v>
       </c>
       <c r="G8" t="n">
-        <v>7.3901</v>
+        <v>-0.4548</v>
       </c>
       <c r="H8" t="n">
-        <v>3.513</v>
+        <v>-0.4093</v>
       </c>
       <c r="I8" t="n">
-        <v>3.5657</v>
+        <v>-0.1929</v>
       </c>
       <c r="J8" t="n">
-        <v>3.635</v>
+        <v>0.041</v>
       </c>
       <c r="K8" t="n">
-        <v>3.6718</v>
+        <v>0.1502</v>
       </c>
       <c r="L8" t="n">
-        <v>3.6962</v>
+        <v>0.2351</v>
       </c>
       <c r="M8" t="n">
-        <v>3.7056</v>
+        <v>0.2242</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>0.1616</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>0.1578</v>
       </c>
     </row>
     <row r="9">
@@ -871,34 +871,34 @@
         <v>0.1311</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0397</v>
+        <v>0.0831</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0535</v>
+        <v>-0.0017</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.2059</v>
+        <v>-0.1921</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0634</v>
+        <v>-0.1241</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0283</v>
+        <v>-0.0635</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0343</v>
+        <v>-0.0528</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0217</v>
+        <v>-0.0243</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0319</v>
+        <v>-0.0345</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0647</v>
+        <v>-0.0673</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0142</v>
+        <v>-0.0571</v>
       </c>
     </row>
     <row r="10">
@@ -918,34 +918,34 @@
         <v>0.1478</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1303</v>
+        <v>0.1281</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0912</v>
+        <v>0.087</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0551</v>
+        <v>0.0507</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.0917</v>
+        <v>-0.0964</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.0805</v>
+        <v>-0.0845</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0958</v>
+        <v>-0.0989</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.0957</v>
+        <v>-0.098</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.0847</v>
+        <v>-0.0865</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.0543</v>
+        <v>-0.0555</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.0522</v>
+        <v>-0.0529</v>
       </c>
     </row>
     <row r="11">
@@ -965,34 +965,34 @@
         <v>0.0139</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0048</v>
+        <v>0.0172</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0044</v>
+        <v>0.0147</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0049</v>
+        <v>0.0123</v>
       </c>
       <c r="I11" t="n">
-        <v>0.005</v>
+        <v>0.0099</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0051</v>
+        <v>0.0099</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0051</v>
+        <v>0.0086</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0054</v>
+        <v>0.0074</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0054</v>
+        <v>0.0074</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0055</v>
+        <v>0.0074</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0054</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="12">
@@ -1012,34 +1012,34 @@
         <v>0.3369</v>
       </c>
       <c r="F12" t="n">
-        <v>-7.9542</v>
+        <v>-0.7867</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.2532</v>
+        <v>-0.2136</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.0975</v>
+        <v>-1.1107</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.725</v>
+        <v>-0.771</v>
       </c>
       <c r="J12" t="n">
-        <v>6.411</v>
+        <v>-0.3653</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.177</v>
+        <v>-0.148</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0505</v>
+        <v>0.109</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0744</v>
+        <v>-0.0033</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0745</v>
+        <v>-0.0739</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.074</v>
+        <v>-0.0585</v>
       </c>
     </row>
     <row r="13">
@@ -1059,34 +1059,34 @@
         <v>0.0321</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.2751</v>
+        <v>-0.0666</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.163</v>
+        <v>-0.1963</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1575</v>
+        <v>-0.1821</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0453</v>
+        <v>-0.0685</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0367</v>
+        <v>-0.0567</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.6114</v>
+        <v>-0.6219</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.6479</v>
+        <v>-0.658</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.3129</v>
+        <v>-0.323</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.1799</v>
+        <v>-0.1988</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.3304</v>
+        <v>-0.3401</v>
       </c>
     </row>
     <row r="14">
@@ -1106,34 +1106,34 @@
         <v>-1.074</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.0879</v>
+        <v>-0.9921</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.48</v>
+        <v>-1.473</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.0322</v>
+        <v>-1.0289</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.4232</v>
+        <v>-0.4205</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.3904</v>
+        <v>-0.4112</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.3008</v>
+        <v>-0.315</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.1495</v>
+        <v>-0.1473</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.0026</v>
+        <v>-0.0049</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0165</v>
+        <v>0.0006</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="15">
@@ -1153,34 +1153,34 @@
         <v>-3.2934</v>
       </c>
       <c r="F15" t="n">
-        <v>-73.9633</v>
+        <v>-2.9551</v>
       </c>
       <c r="G15" t="n">
-        <v>1.934</v>
+        <v>-3.7035</v>
       </c>
       <c r="H15" t="n">
-        <v>-3.6928</v>
+        <v>-3.2729</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.4016</v>
+        <v>-2.096</v>
       </c>
       <c r="J15" t="n">
-        <v>10.7529</v>
+        <v>-1.9671</v>
       </c>
       <c r="K15" t="n">
-        <v>2.911</v>
+        <v>-3.052</v>
       </c>
       <c r="L15" t="n">
-        <v>4.7215</v>
+        <v>-1.131</v>
       </c>
       <c r="M15" t="n">
-        <v>5.198</v>
+        <v>-0.6258</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.3809</v>
+        <v>-1.8299</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.4953</v>
+        <v>-1.1395</v>
       </c>
     </row>
     <row r="16">
@@ -1200,7 +1200,7 @@
         <v>24002.8</v>
       </c>
       <c r="F16" t="n">
-        <v>24188</v>
+        <v>24382.7</v>
       </c>
       <c r="G16" t="n">
         <v>24520.4</v>
@@ -1241,40 +1241,40 @@
         <v>0.5458</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4181</v>
+        <v>-0.0216</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4121</v>
+        <v>0.4228</v>
       </c>
       <c r="F17" t="n">
-        <v>-6.3841</v>
+        <v>0.3908</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.7039</v>
+        <v>-0.1272</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.0169</v>
+        <v>-0.0499</v>
       </c>
       <c r="I17" t="n">
-        <v>3.0568</v>
+        <v>-0.0748</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1055</v>
+        <v>-0.2513</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.3467</v>
+        <v>-0.0846</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.1123</v>
+        <v>-0.1609</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.0284</v>
+        <v>-0.155</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.2212</v>
+        <v>-0.305</v>
       </c>
       <c r="O17" t="n">
-        <v>-0.3622</v>
+        <v>-0.4193</v>
       </c>
     </row>
     <row r="18">
@@ -1341,31 +1341,31 @@
         <v>-1.1757</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.033</v>
+        <v>-0.0334</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.0232</v>
+        <v>-0.0233</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.0345</v>
+        <v>-0.0348</v>
       </c>
       <c r="I19" t="n">
+        <v>-0.0227</v>
+      </c>
+      <c r="J19" t="n">
         <v>-0.0225</v>
       </c>
-      <c r="J19" t="n">
-        <v>-0.0223</v>
-      </c>
       <c r="K19" t="n">
-        <v>-1.0897</v>
+        <v>-1.0899</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.0111</v>
+        <v>-0.0112</v>
       </c>
       <c r="O19" t="n">
         <v>0</v>
@@ -1391,7 +1391,7 @@
         <v>-0.063</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.0288</v>
+        <v>-1.0206</v>
       </c>
       <c r="H20" t="n">
         <v>-0.031</v>
@@ -1429,40 +1429,40 @@
         <v>-0.7397</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.1059</v>
+        <v>0.3339</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.8145</v>
+        <v>-0.8252</v>
       </c>
       <c r="F21" t="n">
-        <v>-36.956</v>
+        <v>-0.7018</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7039</v>
+        <v>0.1004</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0169</v>
+        <v>0.0765</v>
       </c>
       <c r="I21" t="n">
-        <v>-3.0568</v>
+        <v>0.1057</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.1055</v>
+        <v>0.2345</v>
       </c>
       <c r="K21" t="n">
-        <v>0.3467</v>
+        <v>0.0702</v>
       </c>
       <c r="L21" t="n">
-        <v>0.1123</v>
+        <v>0.1488</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0284</v>
+        <v>0.0909</v>
       </c>
       <c r="N21" t="n">
-        <v>0.2212</v>
+        <v>0.2451</v>
       </c>
       <c r="O21" t="n">
-        <v>0.3622</v>
+        <v>-0.2685</v>
       </c>
     </row>
     <row r="22">
@@ -1482,34 +1482,34 @@
         <v>-0.023</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.0163</v>
+        <v>-0.0141</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.0171</v>
+        <v>-0.0143</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.0163</v>
+        <v>-0.0132</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.0158</v>
+        <v>-0.0125</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.0177</v>
+        <v>-0.0142</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0185</v>
+        <v>-0.0148</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.0097</v>
+        <v>-0.0059</v>
       </c>
       <c r="M22" t="n">
-        <v>-0.008</v>
+        <v>-0.0042</v>
       </c>
       <c r="N22" t="n">
-        <v>-0.0041</v>
+        <v>-0.0002</v>
       </c>
       <c r="O22" t="n">
-        <v>-0.0013</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="23">
@@ -1529,34 +1529,34 @@
         <v>0.2154</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.7484</v>
+        <v>0.1111</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.8223</v>
+        <v>0.0898</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.9602</v>
+        <v>-0.002</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.9093</v>
+        <v>0.0085</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.0249</v>
+        <v>0.033</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.0241</v>
+        <v>-0.0495</v>
       </c>
       <c r="L23" t="n">
-        <v>0.012</v>
+        <v>-0.0925</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0017</v>
+        <v>-0.0721</v>
       </c>
       <c r="N23" t="n">
-        <v>0.001</v>
+        <v>-0.0445</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0003</v>
+        <v>-0.0177</v>
       </c>
     </row>
     <row r="24">
@@ -1576,34 +1576,34 @@
         <v>-0.0891</v>
       </c>
       <c r="F24" t="n">
-        <v>4.2624</v>
+        <v>-0.1011</v>
       </c>
       <c r="G24" t="n">
-        <v>4.2267</v>
+        <v>-0.1516</v>
       </c>
       <c r="H24" t="n">
-        <v>2.0944</v>
+        <v>-0.0713</v>
       </c>
       <c r="I24" t="n">
-        <v>2.0469</v>
+        <v>-0.0569</v>
       </c>
       <c r="J24" t="n">
-        <v>2.05</v>
+        <v>-0.0233</v>
       </c>
       <c r="K24" t="n">
-        <v>2.0617</v>
+        <v>0.0159</v>
       </c>
       <c r="L24" t="n">
-        <v>2.0501</v>
+        <v>0.0229</v>
       </c>
       <c r="M24" t="n">
-        <v>2.0466</v>
+        <v>0.0417</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0187</v>
+        <v>0.0641</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>0.0715</v>
       </c>
     </row>
     <row r="25">
@@ -1623,34 +1623,34 @@
         <v>0.0214</v>
       </c>
       <c r="F25" t="n">
-        <v>0.008</v>
+        <v>0.0249</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0084</v>
+        <v>0.0194</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0085</v>
+        <v>0.0171</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0084</v>
+        <v>0.0159</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0083</v>
+        <v>0.0147</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0083</v>
+        <v>0.0135</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0084</v>
+        <v>0.0123</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0082</v>
+        <v>0.0123</v>
       </c>
       <c r="N25" t="n">
-        <v>0.0081</v>
+        <v>0.0111</v>
       </c>
       <c r="O25" t="n">
-        <v>0.0081</v>
+        <v>0.0099</v>
       </c>
     </row>
     <row r="26">
@@ -1670,34 +1670,34 @@
         <v>156.3</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>157.2</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>159.0955</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>161.0138</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>162.9553</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>164.9202</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>166.9088</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>168.9214</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>170.9582</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>173.0196</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>175.1058</v>
       </c>
     </row>
     <row r="27">
@@ -1717,16 +1717,16 @@
         <v>-0.0006</v>
       </c>
       <c r="F27" t="n">
+        <v>-0.0005</v>
+      </c>
+      <c r="G27" t="n">
         <v>-0.001</v>
       </c>
-      <c r="G27" t="n">
-        <v>-0.0009</v>
-      </c>
       <c r="H27" t="n">
-        <v>-0.0005</v>
+        <v>-0.0006</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.0005</v>
+        <v>-0.0006</v>
       </c>
       <c r="J27" t="n">
         <v>-0.0006</v>
@@ -1741,10 +1741,10 @@
         <v>-0.0005</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.0014</v>
+        <v>-0.0015</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.0045</v>
+        <v>-0.0046</v>
       </c>
     </row>
     <row r="28">
@@ -1764,34 +1764,34 @@
         <v>-0.0923</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.1145</v>
+        <v>-0.1281</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.2285</v>
+        <v>-0.2264</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.0842</v>
+        <v>-0.0856</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.0435</v>
+        <v>-0.045</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.0372</v>
+        <v>-0.0356</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.0258</v>
+        <v>-0.0252</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.0145</v>
+        <v>-0.0161</v>
       </c>
       <c r="M28" t="n">
-        <v>-0.0028</v>
+        <v>-0.0036</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.0011</v>
+        <v>0.0002</v>
       </c>
       <c r="O28" t="n">
-        <v>0.0007</v>
+        <v>-0.0002</v>
       </c>
     </row>
     <row r="29">
@@ -1811,34 +1811,34 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>0.0125</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>0.0096</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>0.0072</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>0.0047</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>0.0047</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>0.0034</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>0.0022</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>0.0022</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>0.0022</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="30">
@@ -1858,7 +1858,7 @@
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>13.1667</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1905,34 +1905,34 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>-0.0009</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>-0.0018</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>-0.0016</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>-0.0015</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>-0.0012</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>-0.0011</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>-0.0011</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>-0.0011</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
     </row>
     <row r="32">
@@ -1946,40 +1946,40 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>-0.4397</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>0.0107</v>
       </c>
       <c r="F32" t="n">
-        <v>-32.7296</v>
+        <v>-0.1308</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.316</v>
+        <v>0.1061</v>
       </c>
       <c r="H32" t="n">
-        <v>0.315</v>
+        <v>0.1417</v>
       </c>
       <c r="I32" t="n">
-        <v>3.2108</v>
+        <v>-0.1485</v>
       </c>
       <c r="J32" t="n">
-        <v>0.2054</v>
+        <v>-0.1533</v>
       </c>
       <c r="K32" t="n">
-        <v>0.1772</v>
+        <v>0.2377</v>
       </c>
       <c r="L32" t="n">
-        <v>0.1559</v>
+        <v>-0.0362</v>
       </c>
       <c r="M32" t="n">
-        <v>0.1336</v>
+        <v>-0.1153</v>
       </c>
       <c r="N32" t="n">
-        <v>0.1362</v>
+        <v>-1.4003</v>
       </c>
       <c r="O32" t="n">
-        <v>0.1303</v>
+        <v>-0.0636</v>
       </c>
     </row>
     <row r="33">
@@ -1999,34 +1999,34 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>0.0036</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>0.0045</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>0.0052</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>0.0059</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>0.0064</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>0.0068</v>
       </c>
       <c r="M33" t="n">
-        <v>0</v>
+        <v>0.0071</v>
       </c>
       <c r="N33" t="n">
-        <v>0</v>
+        <v>0.0074</v>
       </c>
       <c r="O33" t="n">
-        <v>0</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="34">
@@ -2046,34 +2046,34 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>-5.355</v>
+        <v>0.0286</v>
       </c>
       <c r="G34" t="n">
-        <v>-5.2609</v>
+        <v>-0.0546</v>
       </c>
       <c r="H34" t="n">
-        <v>-5.1625</v>
+        <v>-0.0406</v>
       </c>
       <c r="I34" t="n">
-        <v>-5.0857</v>
+        <v>-0.066</v>
       </c>
       <c r="J34" t="n">
-        <v>0.1159</v>
+        <v>-0.118</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0823</v>
+        <v>-0.0564</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0724</v>
+        <v>-0.0803</v>
       </c>
       <c r="M34" t="n">
-        <v>0.0189</v>
+        <v>-0.1187</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.0347</v>
+        <v>-0.1043</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0874</v>
+        <v>-0.0903</v>
       </c>
     </row>
     <row r="35">
@@ -2093,34 +2093,34 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>8.0255</v>
+        <v>0.1369</v>
       </c>
       <c r="G35" t="n">
-        <v>8.0629</v>
+        <v>0.218</v>
       </c>
       <c r="H35" t="n">
-        <v>4.1265</v>
+        <v>0.2042</v>
       </c>
       <c r="I35" t="n">
-        <v>3.9589</v>
+        <v>0.2003</v>
       </c>
       <c r="J35" t="n">
-        <v>3.799</v>
+        <v>0.2049</v>
       </c>
       <c r="K35" t="n">
-        <v>3.7324</v>
+        <v>0.2108</v>
       </c>
       <c r="L35" t="n">
-        <v>3.6683</v>
+        <v>0.2071</v>
       </c>
       <c r="M35" t="n">
-        <v>3.6922</v>
+        <v>0.2108</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.0054</v>
+        <v>0.1562</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.0394</v>
+        <v>0.1185</v>
       </c>
     </row>
     <row r="36">
@@ -2140,34 +2140,34 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.1306</v>
+        <v>-0.0077</v>
       </c>
       <c r="G36" t="n">
-        <v>-0.0536</v>
+        <v>-0.0018</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.0172</v>
+        <v>-0.0035</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0599</v>
+        <v>-0.0008</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0332</v>
+        <v>-0.002</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0167</v>
+        <v>-0.0018</v>
       </c>
       <c r="L36" t="n">
+        <v>-0.0017</v>
+      </c>
+      <c r="M36" t="n">
+        <v>-0.0017</v>
+      </c>
+      <c r="N36" t="n">
+        <v>-0.0017</v>
+      </c>
+      <c r="O36" t="n">
         <v>0.0009</v>
-      </c>
-      <c r="M36" t="n">
-        <v>0.0009</v>
-      </c>
-      <c r="N36" t="n">
-        <v>0.0009</v>
-      </c>
-      <c r="O36" t="n">
-        <v>0.0438</v>
       </c>
     </row>
     <row r="37">
@@ -2187,34 +2187,34 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>-0.0022</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>-0.0042</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>-0.0044</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>-0.0047</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>-0.004</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>-0.0031</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>-0.0024</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>-0.0018</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>-0.0011</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>-0.0007</v>
       </c>
     </row>
     <row r="38">
@@ -2234,34 +2234,34 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>0.0123</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>0.0102</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>0.0073</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>0.0048</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>0.0047</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>0.0035</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>0.0019</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>0.0008</v>
       </c>
     </row>
     <row r="39">
@@ -2281,34 +2281,34 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>-7.1645</v>
+        <v>0.0029</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.1794</v>
+        <v>-0.1398</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.1744</v>
+        <v>-0.1876</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.1699</v>
+        <v>-0.2159</v>
       </c>
       <c r="J39" t="n">
-        <v>6.538</v>
+        <v>-0.2384</v>
       </c>
       <c r="K39" t="n">
-        <v>-0.1501</v>
+        <v>-0.1211</v>
       </c>
       <c r="L39" t="n">
-        <v>-0.1472</v>
+        <v>-0.0888</v>
       </c>
       <c r="M39" t="n">
-        <v>-0.1444</v>
+        <v>-0.0733</v>
       </c>
       <c r="N39" t="n">
-        <v>-0.0628</v>
+        <v>-0.0622</v>
       </c>
       <c r="O39" t="n">
-        <v>-0.0616</v>
+        <v>-0.0461</v>
       </c>
     </row>
     <row r="40">
@@ -2328,34 +2328,34 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>-0.1489</v>
+        <v>0.0597</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.014</v>
+        <v>-0.0473</v>
       </c>
       <c r="H40" t="n">
-        <v>-0.0124</v>
+        <v>-0.0371</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0134</v>
+        <v>-0.0098</v>
       </c>
       <c r="J40" t="n">
-        <v>0.0109</v>
+        <v>-0.0091</v>
       </c>
       <c r="K40" t="n">
-        <v>0.0042</v>
+        <v>-0.0062</v>
       </c>
       <c r="L40" t="n">
-        <v>0.0026</v>
+        <v>-0.0075</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0015</v>
+        <v>-0.0086</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0078</v>
+        <v>-0.0112</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0029</v>
+        <v>-0.0069</v>
       </c>
     </row>
     <row r="41">
@@ -2375,34 +2375,34 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.0879</v>
+        <v>0.0079</v>
       </c>
       <c r="G41" t="n">
-        <v>0.014</v>
+        <v>0.0209</v>
       </c>
       <c r="H41" t="n">
+        <v>0.0083</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.0076</v>
+      </c>
+      <c r="J41" t="n">
         <v>0.0051</v>
       </c>
-      <c r="I41" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="J41" t="n">
-        <v>0.0259</v>
-      </c>
       <c r="K41" t="n">
-        <v>0.0171</v>
+        <v>0.0029</v>
       </c>
       <c r="L41" t="n">
+        <v>0.0024</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.0021</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.0006</v>
+      </c>
+      <c r="O41" t="n">
         <v>0.0002</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0.0043</v>
-      </c>
-      <c r="N41" t="n">
-        <v>0.0165</v>
-      </c>
-      <c r="O41" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2422,34 +2422,34 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>-71.828</v>
+        <v>-0.8199</v>
       </c>
       <c r="G42" t="n">
-        <v>5.4196</v>
+        <v>-0.2178</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.4878</v>
+        <v>-0.068</v>
       </c>
       <c r="I42" t="n">
-        <v>-0.3398</v>
+        <v>-0.0341</v>
       </c>
       <c r="J42" t="n">
-        <v>12.8508</v>
+        <v>0.1308</v>
       </c>
       <c r="K42" t="n">
-        <v>6.0023</v>
+        <v>0.0393</v>
       </c>
       <c r="L42" t="n">
-        <v>5.9404</v>
+        <v>0.0878</v>
       </c>
       <c r="M42" t="n">
-        <v>5.8358</v>
+        <v>0.012</v>
       </c>
       <c r="N42" t="n">
-        <v>0.1348</v>
+        <v>-1.3142</v>
       </c>
       <c r="O42" t="n">
-        <v>0.5537</v>
+        <v>-0.0905</v>
       </c>
     </row>
     <row r="43">
@@ -2469,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>194.7</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -2510,40 +2510,40 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>-0.4397</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>0.0107</v>
       </c>
       <c r="F44" t="n">
-        <v>-6.3716</v>
+        <v>0.4033</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.5963</v>
+        <v>-0.0196</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0406</v>
+        <v>0.0077</v>
       </c>
       <c r="I44" t="n">
-        <v>2.9525</v>
+        <v>-0.1791</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0144</v>
+        <v>-0.3424</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0141</v>
+        <v>0.2763</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0143</v>
+        <v>-0.0343</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0133</v>
+        <v>-0.1134</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0128</v>
+        <v>-0.071</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0122</v>
+        <v>-0.0449</v>
       </c>
     </row>
     <row r="45">
@@ -2610,31 +2610,31 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -2660,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>0.0082</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -2698,40 +2698,40 @@
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>0.4397</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>-0.0107</v>
       </c>
       <c r="F48" t="n">
-        <v>-37.0294</v>
+        <v>-0.7752</v>
       </c>
       <c r="G48" t="n">
-        <v>0.3486</v>
+        <v>-0.2549</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.1843</v>
+        <v>-0.1247</v>
       </c>
       <c r="I48" t="n">
-        <v>-2.9482</v>
+        <v>0.2143</v>
       </c>
       <c r="J48" t="n">
-        <v>0.0376</v>
+        <v>0.3776</v>
       </c>
       <c r="K48" t="n">
-        <v>0.0349</v>
+        <v>-0.2416</v>
       </c>
       <c r="L48" t="n">
-        <v>0.0362</v>
+        <v>0.0726</v>
       </c>
       <c r="M48" t="n">
-        <v>0.0261</v>
+        <v>0.0886</v>
       </c>
       <c r="N48" t="n">
-        <v>0.0214</v>
+        <v>0.0452</v>
       </c>
       <c r="O48" t="n">
-        <v>0.5632</v>
+        <v>-0.0674</v>
       </c>
     </row>
     <row r="49">
@@ -2751,34 +2751,34 @@
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>0.0021</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>0.0028</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
+        <v>0.0031</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>0.0033</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
+        <v>0.0036</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>0.0037</v>
       </c>
       <c r="L49" t="n">
-        <v>0</v>
+        <v>0.0038</v>
       </c>
       <c r="M49" t="n">
-        <v>0</v>
+        <v>0.0038</v>
       </c>
       <c r="N49" t="n">
-        <v>0</v>
+        <v>0.0039</v>
       </c>
       <c r="O49" t="n">
-        <v>0</v>
+        <v>0.0039</v>
       </c>
     </row>
     <row r="50">
@@ -2798,34 +2798,34 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.928</v>
+        <v>-0.0684</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.9241</v>
+        <v>-0.0119</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.9754</v>
+        <v>-0.0172</v>
       </c>
       <c r="I50" t="n">
-        <v>-0.9395</v>
+        <v>-0.0217</v>
       </c>
       <c r="J50" t="n">
-        <v>-0.0183</v>
+        <v>0.0395</v>
       </c>
       <c r="K50" t="n">
-        <v>0.007</v>
+        <v>-0.0185</v>
       </c>
       <c r="L50" t="n">
-        <v>0.09</v>
+        <v>-0.0145</v>
       </c>
       <c r="M50" t="n">
-        <v>0.062</v>
+        <v>-0.0118</v>
       </c>
       <c r="N50" t="n">
-        <v>0.0364</v>
+        <v>-0.0091</v>
       </c>
       <c r="O50" t="n">
-        <v>0.0113</v>
+        <v>-0.0067</v>
       </c>
     </row>
     <row r="51">
@@ -2845,34 +2845,34 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>4.3134</v>
+        <v>-0.0501</v>
       </c>
       <c r="G51" t="n">
-        <v>4.3316</v>
+        <v>-0.0467</v>
       </c>
       <c r="H51" t="n">
-        <v>2.1745</v>
+        <v>0.0088</v>
       </c>
       <c r="I51" t="n">
-        <v>2.1326</v>
+        <v>0.0288</v>
       </c>
       <c r="J51" t="n">
-        <v>2.1072</v>
+        <v>0.0339</v>
       </c>
       <c r="K51" t="n">
-        <v>2.0846</v>
+        <v>0.0387</v>
       </c>
       <c r="L51" t="n">
-        <v>2.0652</v>
+        <v>0.038</v>
       </c>
       <c r="M51" t="n">
-        <v>2.0448</v>
+        <v>0.04</v>
       </c>
       <c r="N51" t="n">
-        <v>0.0228</v>
+        <v>0.0681</v>
       </c>
       <c r="O51" t="n">
-        <v>-0.005</v>
+        <v>0.0665</v>
       </c>
     </row>
     <row r="52">
@@ -2892,34 +2892,34 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>0.0169</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>0.0111</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>0.0086</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>0.0075</v>
       </c>
       <c r="J52" t="n">
-        <v>0</v>
+        <v>0.0063</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>0.0052</v>
       </c>
       <c r="L52" t="n">
-        <v>0</v>
+        <v>0.0039</v>
       </c>
       <c r="M52" t="n">
-        <v>0</v>
+        <v>0.0041</v>
       </c>
       <c r="N52" t="n">
-        <v>0</v>
+        <v>0.0029</v>
       </c>
       <c r="O52" t="n">
-        <v>0</v>
+        <v>0.0018</v>
       </c>
     </row>
     <row r="53">
@@ -2939,34 +2939,34 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>-158.1846</v>
+        <v>-0.9846</v>
       </c>
       <c r="G53" t="n">
-        <v>-160.092</v>
+        <v>-0.9965</v>
       </c>
       <c r="H53" t="n">
-        <v>-162.0224</v>
+        <v>-1.0085</v>
       </c>
       <c r="I53" t="n">
-        <v>-163.976</v>
+        <v>-1.0207</v>
       </c>
       <c r="J53" t="n">
-        <v>-165.9532</v>
+        <v>-1.033</v>
       </c>
       <c r="K53" t="n">
-        <v>-167.9542</v>
+        <v>-1.0455</v>
       </c>
       <c r="L53" t="n">
-        <v>-169.9794</v>
+        <v>-1.0581</v>
       </c>
       <c r="M53" t="n">
-        <v>-172.029</v>
+        <v>-1.0708</v>
       </c>
       <c r="N53" t="n">
-        <v>-174.1033</v>
+        <v>-1.0837</v>
       </c>
       <c r="O53" t="n">
-        <v>-176.2026</v>
+        <v>-1.0968</v>
       </c>
     </row>
     <row r="54">
@@ -2986,10 +2986,10 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>0.0006</v>
       </c>
       <c r="G54" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -3033,34 +3033,34 @@
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>-0.0137</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>0.0021</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>-0.0014</v>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>-0.0015</v>
       </c>
       <c r="J55" t="n">
-        <v>0</v>
+        <v>0.0016</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
+        <v>0.0006</v>
       </c>
       <c r="L55" t="n">
-        <v>0</v>
+        <v>-0.0016</v>
       </c>
       <c r="M55" t="n">
-        <v>0</v>
+        <v>-0.0008</v>
       </c>
       <c r="N55" t="n">
-        <v>0</v>
+        <v>0.0012</v>
       </c>
       <c r="O55" t="n">
-        <v>0</v>
+        <v>-0.0009</v>
       </c>
     </row>
     <row r="56">

</xml_diff>